<commit_message>
Upgraded leaderboards with position change
</commit_message>
<xml_diff>
--- a/Bot_screening/correlation.xlsx
+++ b/Bot_screening/correlation.xlsx
@@ -477,12 +477,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cardano</t>
+          <t>ripple</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>ripple</t>
+          <t>cardano</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -498,223 +498,223 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44780</v>
+        <v>44781</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3588927774862672</v>
+        <v>0.3347276281545201</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.8180411302471682</v>
+        <v>-1</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.8710817171148656</v>
+        <v>-0.998485803379483</v>
       </c>
       <c r="F2" t="n">
-        <v>1.989130950673117</v>
+        <v>-0.7591963399247146</v>
       </c>
       <c r="G2" t="n">
         <v>-1</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.2852520880129226</v>
+        <v>-0.3708805448826741</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.8174832039608152</v>
+        <v>-0.7182598828266793</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3051725216229448</v>
+        <v>0.329693983977981</v>
       </c>
       <c r="K2" t="n">
-        <v>2.812878852257569</v>
+        <v>1.249565521564594</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44781</v>
+        <v>44782</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08728662200221803</v>
+        <v>0.5663835326339063</v>
       </c>
       <c r="D3" t="n">
         <v>-1</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.013030811599958</v>
+        <v>-1</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.7213085191880166</v>
+        <v>-0.4491192622160226</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.9730233937773972</v>
+        <v>-1</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.290733645129098</v>
+        <v>0.1189413924176802</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.5800665665759893</v>
+        <v>0.5182890457867533</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2170516419272841</v>
+        <v>0.5140003965507199</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7620011316656453</v>
+        <v>0.3872089747513092</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44782</v>
+        <v>44783</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5663835326339063</v>
+        <v>2.439499444527764</v>
       </c>
       <c r="D4" t="n">
-        <v>-1</v>
+        <v>-1.003848286446325</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.4491192622160226</v>
+        <v>0.02785428587696061</v>
       </c>
       <c r="G4" t="n">
-        <v>-1</v>
+        <v>-1.216885477154323</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5182890457867533</v>
+        <v>0.3005265642412925</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1189413924176802</v>
+        <v>0.7233996580738042</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5140003965507199</v>
+        <v>0.3480056208222438</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3872089747513092</v>
+        <v>2.872870756341862</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44783</v>
+        <v>44784</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>2.439499444527764</v>
+        <v>0.6177808690255379</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.003848286446325</v>
+        <v>-1.004615248843157</v>
       </c>
       <c r="E5" t="n">
-        <v>-1</v>
+        <v>-1.03401438397407</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02785428587696061</v>
+        <v>-1.122794779459527</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.216885477154323</v>
+        <v>-1.033783621531911</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7233996580738042</v>
+        <v>-0.646738122174017</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3005265642412925</v>
+        <v>-0.7523542407950966</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3480056208222438</v>
+        <v>1.153634010467608</v>
       </c>
       <c r="K5" t="n">
-        <v>2.872870756341862</v>
+        <v>-2.353161964485982</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44784</v>
+        <v>44785</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6177808690255379</v>
+        <v>3.406652427755102</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.004615248843157</v>
+        <v>-1</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.03401438397407</v>
+        <v>-2.228995538443294</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.122794779459527</v>
+        <v>-3.421127529043298</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.033783621531911</v>
+        <v>-0.8538647142988285</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.7523542407950966</v>
+        <v>-7.403187282051323</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.646738122174017</v>
+        <v>0.3704768852221876</v>
       </c>
       <c r="J6" t="n">
-        <v>1.153634010467608</v>
+        <v>2.279580427915934</v>
       </c>
       <c r="K6" t="n">
-        <v>-2.353161964485982</v>
+        <v>5.325686832042503</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44785</v>
+        <v>44786</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3.406652427755102</v>
+        <v>1.842211083576082</v>
       </c>
       <c r="D7" t="n">
         <v>-1</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.228995538443294</v>
+        <v>-1</v>
       </c>
       <c r="F7" t="n">
-        <v>-3.421127529043298</v>
+        <v>-0.7521637708165091</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.8538647142988285</v>
+        <v>-0.9292297166892991</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3704768852221876</v>
+        <v>-0.3282015246135956</v>
       </c>
       <c r="I7" t="n">
-        <v>-7.403187282051323</v>
+        <v>2.256300637166398</v>
       </c>
       <c r="J7" t="n">
-        <v>2.279580427915934</v>
+        <v>3.496265916212682</v>
       </c>
       <c r="K7" t="n">
-        <v>5.325686832042503</v>
+        <v>-0.8929529026018798</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44786</v>
+        <v>44787</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1.842211083576082</v>
+        <v>2.580229989822237</v>
       </c>
       <c r="D8" t="n">
         <v>-1</v>
@@ -723,33 +723,33 @@
         <v>-1</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.7521637708165091</v>
+        <v>1.373210348983618</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.9292297166892991</v>
+        <v>-1</v>
       </c>
       <c r="H8" t="n">
-        <v>2.256300637166398</v>
+        <v>-1.206127526617662</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.3282015246135956</v>
+        <v>-3.75550241621478</v>
       </c>
       <c r="J8" t="n">
-        <v>3.496265916212682</v>
+        <v>3.363920145033541</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.8929529026018798</v>
+        <v>5.115802273544364</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44787</v>
+        <v>44788</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2.580229989822237</v>
+        <v>1.504715626190854</v>
       </c>
       <c r="D9" t="n">
         <v>-1</v>
@@ -758,348 +758,348 @@
         <v>-1</v>
       </c>
       <c r="F9" t="n">
-        <v>1.373210348983618</v>
+        <v>-0.7396241317340134</v>
       </c>
       <c r="G9" t="n">
         <v>-1</v>
       </c>
       <c r="H9" t="n">
-        <v>-3.75550241621478</v>
+        <v>1.912466267395957</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.206127526617662</v>
+        <v>1.336769811251976</v>
       </c>
       <c r="J9" t="n">
-        <v>3.363920145033541</v>
+        <v>2.743975281793704</v>
       </c>
       <c r="K9" t="n">
-        <v>5.115802273544364</v>
+        <v>1.164467534568431</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44788</v>
+        <v>44789</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1.504715626190854</v>
+        <v>0.3557951604305785</v>
       </c>
       <c r="D10" t="n">
         <v>-1</v>
       </c>
       <c r="E10" t="n">
-        <v>-1</v>
+        <v>-0.9661402886512506</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.7396241317340134</v>
+        <v>0.4009431948855561</v>
       </c>
       <c r="G10" t="n">
-        <v>-1</v>
+        <v>-0.6538409321937547</v>
       </c>
       <c r="H10" t="n">
-        <v>1.336769811251976</v>
+        <v>-0.9181934766978933</v>
       </c>
       <c r="I10" t="n">
-        <v>1.912466267395957</v>
+        <v>-1.317202453889554</v>
       </c>
       <c r="J10" t="n">
-        <v>2.743975281793704</v>
+        <v>1.052166178521591</v>
       </c>
       <c r="K10" t="n">
-        <v>1.164467534568431</v>
+        <v>-0.4721718220402626</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44789</v>
+        <v>44790</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3557951604305785</v>
+        <v>-0.3493480933411094</v>
       </c>
       <c r="D11" t="n">
         <v>-1</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.9661402886512506</v>
+        <v>-1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4009431948855561</v>
+        <v>-0.113048456370309</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.6538409321937547</v>
+        <v>-1</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.317202453889554</v>
+        <v>-1.482094813239377</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.9181934766978933</v>
+        <v>0.9529344026279107</v>
       </c>
       <c r="J11" t="n">
-        <v>1.052166178521591</v>
+        <v>1.134838649104895</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.4721718220402626</v>
+        <v>1.290790950721509</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44790</v>
+        <v>44791</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.3493480933411094</v>
+        <v>-17.38643511365984</v>
       </c>
       <c r="D12" t="n">
-        <v>-1</v>
+        <v>0.6974339439449682</v>
       </c>
       <c r="E12" t="n">
-        <v>-1</v>
+        <v>-1.50684981924193</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.113048456370309</v>
+        <v>21.35318887889001</v>
       </c>
       <c r="G12" t="n">
         <v>-1</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9529344026279107</v>
+        <v>9.613714896813168</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.482094813239377</v>
+        <v>24.27166700282406</v>
       </c>
       <c r="J12" t="n">
-        <v>1.134838649104895</v>
+        <v>7.755431615760426</v>
       </c>
       <c r="K12" t="n">
-        <v>1.290790950721509</v>
+        <v>9.235979507099051</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44791</v>
+        <v>44792</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>-17.38643511365984</v>
+        <v>0.07182946629507683</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6974339439449682</v>
+        <v>-1</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.50684981924193</v>
+        <v>-1.002459396999817</v>
       </c>
       <c r="F13" t="n">
-        <v>21.35318887889001</v>
+        <v>-0.3137476012172053</v>
       </c>
       <c r="G13" t="n">
-        <v>-1</v>
+        <v>-1.009737700108099</v>
       </c>
       <c r="H13" t="n">
-        <v>24.27166700282406</v>
+        <v>0.1979516449373755</v>
       </c>
       <c r="I13" t="n">
-        <v>9.613714896813168</v>
+        <v>0.4001310478555686</v>
       </c>
       <c r="J13" t="n">
-        <v>7.755431615760426</v>
+        <v>0.03969682276691847</v>
       </c>
       <c r="K13" t="n">
-        <v>9.235979507099051</v>
+        <v>0.2605346817380879</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44792</v>
+        <v>44793</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07182946629507683</v>
+        <v>7.093562642850708</v>
       </c>
       <c r="D14" t="n">
         <v>-1</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.002459396999817</v>
+        <v>-1</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.3137476012172053</v>
+        <v>1.018916478382335</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.009737700108099</v>
+        <v>-0.9222199119266031</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4001310478555686</v>
+        <v>0.8605713498406516</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1979516449373755</v>
+        <v>4.900282768426139</v>
       </c>
       <c r="J14" t="n">
-        <v>0.03969682276691847</v>
+        <v>4.002828378026852</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2605346817380879</v>
+        <v>2.79639606710775</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44793</v>
+        <v>44794</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>7.093562642850708</v>
+        <v>0.5708347656348998</v>
       </c>
       <c r="D15" t="n">
-        <v>-1</v>
+        <v>-0.9965650581183695</v>
       </c>
       <c r="E15" t="n">
-        <v>-1</v>
+        <v>-0.9702022668214413</v>
       </c>
       <c r="F15" t="n">
-        <v>1.018916478382335</v>
+        <v>1.857973302001843</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.9222199119266031</v>
+        <v>-1</v>
       </c>
       <c r="H15" t="n">
-        <v>4.900282768426139</v>
+        <v>-0.01828439981603385</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8605713498406516</v>
+        <v>1.34599443546372</v>
       </c>
       <c r="J15" t="n">
-        <v>4.002828378026852</v>
+        <v>1.386451942795941</v>
       </c>
       <c r="K15" t="n">
-        <v>2.79639606710775</v>
+        <v>0.680251303779754</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44794</v>
+        <v>44795</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5708347656348998</v>
+        <v>0.7930527782615641</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.9965650581183695</v>
+        <v>-1</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.9702022668214413</v>
+        <v>-1.01247428964044</v>
       </c>
       <c r="F16" t="n">
-        <v>1.857973302001843</v>
+        <v>-0.271351547833475</v>
       </c>
       <c r="G16" t="n">
-        <v>-1</v>
+        <v>-0.8483519749421524</v>
       </c>
       <c r="H16" t="n">
-        <v>1.34599443546372</v>
+        <v>0.2711831224757774</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.01828439981603385</v>
+        <v>0.8010554006067262</v>
       </c>
       <c r="J16" t="n">
-        <v>1.386451942795941</v>
+        <v>1.54903645392441</v>
       </c>
       <c r="K16" t="n">
-        <v>0.680251303779754</v>
+        <v>0.4873779841139315</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44795</v>
+        <v>44796</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7930527782615641</v>
+        <v>1.553897911160715</v>
       </c>
       <c r="D17" t="n">
         <v>-1</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.01247428964044</v>
+        <v>-1.045945165766393</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.271351547833475</v>
+        <v>-0.5459832130735258</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.8483519749421524</v>
+        <v>-1</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8010554006067262</v>
+        <v>0.3150234949132837</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2711831224757774</v>
+        <v>0.07646887553552671</v>
       </c>
       <c r="J17" t="n">
-        <v>1.54903645392441</v>
+        <v>0.1938343926459315</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4873779841139315</v>
+        <v>1.4948227335873</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44796</v>
+        <v>44797</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>1.553897911160715</v>
+        <v>0.6760245499330867</v>
       </c>
       <c r="D18" t="n">
         <v>-1</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.045945165766393</v>
+        <v>-1</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.5459832130735258</v>
+        <v>-1.072577873573307</v>
       </c>
       <c r="G18" t="n">
         <v>-1</v>
       </c>
       <c r="H18" t="n">
-        <v>0.07646887553552671</v>
+        <v>-0.2254990028970178</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3150234949132837</v>
+        <v>-0.3074984866650995</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1938343926459315</v>
+        <v>0.7454905578412521</v>
       </c>
       <c r="K18" t="n">
-        <v>1.4948227335873</v>
+        <v>0.0151526016278579</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44797</v>
+        <v>44798</v>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6760245499330867</v>
+        <v>-2.226252406890069</v>
       </c>
       <c r="D19" t="n">
         <v>-1</v>
@@ -1108,33 +1108,33 @@
         <v>-1</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.072577873573307</v>
+        <v>-1.783573586938949</v>
       </c>
       <c r="G19" t="n">
         <v>-1</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.3074984866650995</v>
+        <v>-0.4305916218935319</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.2254990028970178</v>
+        <v>-0.9767483865732541</v>
       </c>
       <c r="J19" t="n">
-        <v>0.7454905578412521</v>
+        <v>0.02586844363957861</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0151526016278579</v>
+        <v>1.176488303683986</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44798</v>
+        <v>44799</v>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>-2.226252406890069</v>
+        <v>1.056872289430486</v>
       </c>
       <c r="D20" t="n">
         <v>-1</v>
@@ -1143,348 +1143,348 @@
         <v>-1</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.783573586938949</v>
+        <v>0.343212637543868</v>
       </c>
       <c r="G20" t="n">
         <v>-1</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.9767483865732541</v>
+        <v>-0.1966202771200968</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.4305916218935319</v>
+        <v>0.1457270014357791</v>
       </c>
       <c r="J20" t="n">
-        <v>0.02586844363957861</v>
+        <v>0.8537729983577181</v>
       </c>
       <c r="K20" t="n">
-        <v>1.176488303683986</v>
+        <v>0.5108596544767</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44799</v>
+        <v>44800</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>1.056872289430486</v>
+        <v>0.7447545595670189</v>
       </c>
       <c r="D21" t="n">
-        <v>-1</v>
+        <v>-1.000353162969686</v>
       </c>
       <c r="E21" t="n">
-        <v>-1</v>
+        <v>-0.9994699321639933</v>
       </c>
       <c r="F21" t="n">
-        <v>0.343212637543868</v>
+        <v>-0.1424242657032674</v>
       </c>
       <c r="G21" t="n">
-        <v>-1</v>
+        <v>-0.9957037166740248</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1457270014357791</v>
+        <v>-0.497125676871547</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.1966202771200968</v>
+        <v>-0.9385055924429726</v>
       </c>
       <c r="J21" t="n">
-        <v>0.8537729983577181</v>
+        <v>0.7204887724212452</v>
       </c>
       <c r="K21" t="n">
-        <v>0.5108596544767</v>
+        <v>-0.5033485548840178</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44800</v>
+        <v>44801</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7447545595670189</v>
+        <v>58.36234144067808</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.000353162969686</v>
+        <v>1.396297292901451</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.9994699321639933</v>
+        <v>2.216103642050449</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.1424242657032674</v>
+        <v>96.303128455497</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.9957037166740248</v>
+        <v>-1</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.9385055924429726</v>
+        <v>8.735623693222541</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.497125676871547</v>
+        <v>11.02421443058655</v>
       </c>
       <c r="J22" t="n">
-        <v>0.7204887724212452</v>
+        <v>119.6864362497556</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.5033485548840178</v>
+        <v>57.66632497657236</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44801</v>
+        <v>44802</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>58.36234144067808</v>
+        <v>2.167285783005582</v>
       </c>
       <c r="D23" t="n">
-        <v>1.396297292901451</v>
+        <v>-1</v>
       </c>
       <c r="E23" t="n">
-        <v>2.216103642050449</v>
+        <v>-1.032846784698916</v>
       </c>
       <c r="F23" t="n">
-        <v>96.303128455497</v>
+        <v>-1.140052524619962</v>
       </c>
       <c r="G23" t="n">
         <v>-1</v>
       </c>
       <c r="H23" t="n">
-        <v>11.02421443058655</v>
+        <v>-2.990924550964826</v>
       </c>
       <c r="I23" t="n">
-        <v>8.735623693222541</v>
+        <v>-0.1217418524199236</v>
       </c>
       <c r="J23" t="n">
-        <v>119.6864362497556</v>
+        <v>-1.248695853992646</v>
       </c>
       <c r="K23" t="n">
-        <v>57.66632497657236</v>
+        <v>0.3951767056553147</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44802</v>
+        <v>44803</v>
       </c>
       <c r="B24" t="n">
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>2.167285783005582</v>
+        <v>0.0282790850066271</v>
       </c>
       <c r="D24" t="n">
-        <v>-1</v>
+        <v>-1.017401247346963</v>
       </c>
       <c r="E24" t="n">
-        <v>-1.032846784698916</v>
+        <v>-1</v>
       </c>
       <c r="F24" t="n">
-        <v>-1.140052524619962</v>
+        <v>-0.5420080328412906</v>
       </c>
       <c r="G24" t="n">
-        <v>-1</v>
+        <v>-1.116211758790248</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.1217418524199236</v>
+        <v>0.1448738385337185</v>
       </c>
       <c r="I24" t="n">
-        <v>-2.990924550964826</v>
+        <v>-0.4528069410873235</v>
       </c>
       <c r="J24" t="n">
-        <v>-1.248695853992646</v>
+        <v>-0.2438170218950537</v>
       </c>
       <c r="K24" t="n">
-        <v>0.3951767056553147</v>
+        <v>0.7518266746672676</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44803</v>
+        <v>44804</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0282790850066271</v>
+        <v>0.3821874927678333</v>
       </c>
       <c r="D25" t="n">
-        <v>-1.017401247346963</v>
+        <v>-1</v>
       </c>
       <c r="E25" t="n">
         <v>-1</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.5420080328412906</v>
+        <v>-19.32853690482652</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.116211758790248</v>
+        <v>-1</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.4528069410873235</v>
+        <v>-3.677799148078235</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1448738385337185</v>
+        <v>-2.964066549511795</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.2438170218950537</v>
+        <v>4.32658903822204</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7518266746672676</v>
+        <v>1.393938596155473</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44804</v>
+        <v>44805</v>
       </c>
       <c r="B26" t="n">
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>0.3821874927678333</v>
+        <v>-0.4812085633661006</v>
       </c>
       <c r="D26" t="n">
-        <v>-1</v>
+        <v>-1.107856478988109</v>
       </c>
       <c r="E26" t="n">
-        <v>-1</v>
+        <v>-1.090990496397297</v>
       </c>
       <c r="F26" t="n">
-        <v>-19.32853690482652</v>
+        <v>0.3542251761722357</v>
       </c>
       <c r="G26" t="n">
-        <v>-1</v>
+        <v>-1.00348981024844</v>
       </c>
       <c r="H26" t="n">
-        <v>-2.964066549511795</v>
+        <v>-0.6899035308803454</v>
       </c>
       <c r="I26" t="n">
-        <v>-3.677799148078235</v>
+        <v>-1.017728337994833</v>
       </c>
       <c r="J26" t="n">
-        <v>4.32658903822204</v>
+        <v>1.104019666264315</v>
       </c>
       <c r="K26" t="n">
-        <v>1.393938596155473</v>
+        <v>-0.4707024078998651</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44805</v>
+        <v>44806</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.4812085633661006</v>
+        <v>0.6439846298355287</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.107856478988109</v>
+        <v>-0.9955447196426502</v>
       </c>
       <c r="E27" t="n">
-        <v>-1.090990496397297</v>
+        <v>-1</v>
       </c>
       <c r="F27" t="n">
-        <v>0.3542251761722357</v>
+        <v>0.2784347103415837</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.00348981024844</v>
+        <v>-1</v>
       </c>
       <c r="H27" t="n">
-        <v>-1.017728337994833</v>
+        <v>-1.462764912319961</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.6899035308803454</v>
+        <v>-0.3272974087900659</v>
       </c>
       <c r="J27" t="n">
-        <v>1.104019666264315</v>
+        <v>-0.1477970161575379</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.4707024078998651</v>
+        <v>5.71430340446416</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44806</v>
+        <v>44807</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6439846298355287</v>
+        <v>-0.5015060938193778</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.9955447196426502</v>
+        <v>-1.130203289196921</v>
       </c>
       <c r="E28" t="n">
-        <v>-1</v>
+        <v>-1.114133833239052</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2784347103415837</v>
+        <v>-2.642540151023747</v>
       </c>
       <c r="G28" t="n">
-        <v>-1</v>
+        <v>-0.8912278466966744</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.3272974087900659</v>
+        <v>-3.388876056682919</v>
       </c>
       <c r="I28" t="n">
-        <v>-1.462764912319961</v>
+        <v>-15.21259706852648</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.1477970161575379</v>
+        <v>-1.983452609227662</v>
       </c>
       <c r="K28" t="n">
-        <v>5.71430340446416</v>
+        <v>-0.4422155388724135</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44807</v>
+        <v>44808</v>
       </c>
       <c r="B29" t="n">
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.5015060938193778</v>
+        <v>0.9790192988206247</v>
       </c>
       <c r="D29" t="n">
-        <v>-1.130203289196921</v>
+        <v>-1</v>
       </c>
       <c r="E29" t="n">
-        <v>-1.114133833239052</v>
+        <v>-1</v>
       </c>
       <c r="F29" t="n">
-        <v>-2.642540151023747</v>
+        <v>0.3601190733038876</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.8912278466966744</v>
+        <v>-1</v>
       </c>
       <c r="H29" t="n">
-        <v>-15.21259706852648</v>
+        <v>-0.2580650170860813</v>
       </c>
       <c r="I29" t="n">
-        <v>-3.388876056682919</v>
+        <v>10.19879112603133</v>
       </c>
       <c r="J29" t="n">
-        <v>-1.983452609227662</v>
+        <v>4.582448118657625</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.4422155388724135</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44808</v>
+        <v>44809</v>
       </c>
       <c r="B30" t="n">
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0.9790192988206247</v>
+        <v>-2.413039666084244</v>
       </c>
       <c r="D30" t="n">
         <v>-1</v>
@@ -1493,92 +1493,92 @@
         <v>-1</v>
       </c>
       <c r="F30" t="n">
-        <v>0.3601190733038876</v>
+        <v>0.2205708710846189</v>
       </c>
       <c r="G30" t="n">
         <v>-1</v>
       </c>
       <c r="H30" t="n">
-        <v>10.19879112603133</v>
+        <v>-0.35959016278294</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.2580650170860813</v>
+        <v>1.459952992033018</v>
       </c>
       <c r="J30" t="n">
-        <v>4.582448118657625</v>
+        <v>-1.368076912450871</v>
       </c>
       <c r="K30" t="n">
-        <v>-1</v>
+        <v>-1.893330485972785</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44809</v>
+        <v>44810</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>-2.413039666084244</v>
+        <v>-0.7674276358826986</v>
       </c>
       <c r="D31" t="n">
-        <v>-1</v>
+        <v>-0.9746379203969708</v>
       </c>
       <c r="E31" t="n">
-        <v>-1</v>
+        <v>-0.9589154930007838</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2205708710846189</v>
+        <v>-0.1220077777212775</v>
       </c>
       <c r="G31" t="n">
-        <v>-1</v>
+        <v>-0.9651786894881172</v>
       </c>
       <c r="H31" t="n">
-        <v>1.459952992033018</v>
+        <v>-0.4147765128364558</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.35959016278294</v>
+        <v>0.04029869248277464</v>
       </c>
       <c r="J31" t="n">
-        <v>-1.368076912450871</v>
+        <v>-0.2944056043762592</v>
       </c>
       <c r="K31" t="n">
-        <v>-1.893330485972785</v>
+        <v>0.09753929310439116</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44810</v>
+        <v>44811</v>
       </c>
       <c r="B32" t="n">
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>4.592304794513248</v>
+        <v>-0.2232429467187066</v>
       </c>
       <c r="D32" t="n">
-        <v>-1.001446258426337</v>
+        <v>-1.012214078299195</v>
       </c>
       <c r="E32" t="n">
-        <v>-1</v>
+        <v>-0.6439846762858801</v>
       </c>
       <c r="F32" t="n">
-        <v>1.897996700973304</v>
+        <v>-1.73412942444457</v>
       </c>
       <c r="G32" t="n">
-        <v>-1</v>
+        <v>0.2502479967898074</v>
       </c>
       <c r="H32" t="n">
-        <v>1.435949915418238</v>
+        <v>-0.627698834749752</v>
       </c>
       <c r="I32" t="n">
-        <v>0.8297228330562624</v>
+        <v>-1.100547546225384</v>
       </c>
       <c r="J32" t="n">
-        <v>4.075942097552542</v>
+        <v>-0.2140232754699785</v>
       </c>
       <c r="K32" t="n">
-        <v>4.1957720303595</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged the screening coins files
</commit_message>
<xml_diff>
--- a/Bot_screening/correlation.xlsx
+++ b/Bot_screening/correlation.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -514,16 +514,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6438720181551419</v>
+        <v>0.1513560054718786</v>
       </c>
       <c r="D2" t="n">
-        <v>-11.06008232959217</v>
+        <v>-6.294687658057581</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>-6.294687658057581</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2445906649195572</v>
+        <v>-0.8269167698135087</v>
       </c>
       <c r="G2" t="n">
         <v>-1</v>
@@ -532,19 +532,19 @@
         <v>-1</v>
       </c>
       <c r="I2" t="n">
-        <v>20.37767495038343</v>
+        <v>10.2512112733724</v>
       </c>
       <c r="J2" t="n">
-        <v>7.485794636793413</v>
+        <v>-0.1524511281828686</v>
       </c>
       <c r="K2" t="n">
         <v>-1</v>
       </c>
       <c r="L2" t="n">
-        <v>-1</v>
+        <v>-0.2622156542051112</v>
       </c>
       <c r="M2" t="n">
-        <v>17.17618739742738</v>
+        <v>8.566247266248954</v>
       </c>
     </row>
     <row r="3">
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.4150175407439368</v>
+        <v>-0.5024491423859256</v>
       </c>
       <c r="D32" t="n">
         <v>-1</v>
@@ -1753,10 +1753,10 @@
         <v>-1</v>
       </c>
       <c r="F32" t="n">
-        <v>-1.86727630754145</v>
+        <v>-1.348648551689004</v>
       </c>
       <c r="G32" t="n">
-        <v>17.42270846323888</v>
+        <v>5.534708212411552</v>
       </c>
       <c r="H32" t="n">
         <v>-1</v>
@@ -1765,13 +1765,13 @@
         <v>-1</v>
       </c>
       <c r="J32" t="n">
-        <v>0.007064277253669342</v>
+        <v>-0.8213924077415695</v>
       </c>
       <c r="K32" t="n">
         <v>-1</v>
       </c>
       <c r="L32" t="n">
-        <v>1.615569720089462</v>
+        <v>-1</v>
       </c>
       <c r="M32" t="n">
         <v>-1</v>

</xml_diff>